<commit_message>
updated Wildcard matrix and Eventghost regression test cases
</commit_message>
<xml_diff>
--- a/Testen/WildCard matrix.xlsx
+++ b/Testen/WildCard matrix.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
   <si>
     <t>WildCard matrix</t>
   </si>
@@ -51,9 +51,6 @@
     <t>System</t>
   </si>
   <si>
-    <t>Command</t>
-  </si>
-  <si>
     <t>Event</t>
   </si>
   <si>
@@ -88,28 +85,12 @@
   </si>
   <si>
     <t>onduidelijk, heeft uitleg nodig, of testcase onduidelijk</t>
-  </si>
-  <si>
-    <t>16,12
-inkomend commando vanuit andere unit</t>
   </si>
   <si>
     <t xml:space="preserve">16,13
 inkomend signaal </t>
   </si>
   <si>
-    <t>16,22
-inkomend commando vanuit andere unit</t>
-  </si>
-  <si>
-    <t>16,32
-EventGhost stuurt command</t>
-  </si>
-  <si>
-    <t>16,82
-kan ik een commando vanuit de EventList afvuren?</t>
-  </si>
-  <si>
     <t xml:space="preserve">16,23
 inkomend signaal </t>
   </si>
@@ -134,18 +115,6 @@
 variable wijzigt waarde</t>
   </si>
   <si>
-    <t>16,83
-UserEvent??</t>
-  </si>
-  <si>
-    <t>16,93
-??</t>
-  </si>
-  <si>
-    <t>16,92
-??</t>
-  </si>
-  <si>
     <t>16,25
 inkomend signaal, maar bestemd voor andere unit</t>
   </si>
@@ -155,6 +124,30 @@
   <si>
     <t>16,15
 inkomend signaal, maar bestemd voor andere unit</t>
+  </si>
+  <si>
+    <t>16,84
+hex value uit eventlist</t>
+  </si>
+  <si>
+    <t>16,83
+UserEvent</t>
+  </si>
+  <si>
+    <t>16,93
+boot</t>
+  </si>
+  <si>
+    <t>16,14
+inkomend signaal</t>
+  </si>
+  <si>
+    <t>16,24
+hex value uit RF</t>
+  </si>
+  <si>
+    <t>16,34
+hex value uit Serial</t>
   </si>
 </sst>
 </file>
@@ -322,15 +315,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -349,15 +339,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -379,12 +360,6 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -398,6 +373,12 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -704,7 +685,7 @@
   <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -713,18 +694,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -740,27 +721,21 @@
       <c r="E6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>14</v>
-      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="13">
+      <c r="B7" s="9">
         <v>16.100000000000001</v>
       </c>
-      <c r="C7" s="20">
-        <v>16.2</v>
-      </c>
-      <c r="D7" s="15">
+      <c r="C7" s="11">
         <v>16.3</v>
       </c>
-      <c r="E7" s="21">
+      <c r="D7" s="11">
         <v>16.399999999999999</v>
       </c>
-      <c r="F7" s="22">
+      <c r="E7" s="16">
         <v>16.5</v>
       </c>
       <c r="G7" s="2"/>
@@ -770,59 +745,50 @@
       <c r="A8" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="16">
+      <c r="B8" s="12">
         <v>16.11</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="E8" s="19">
-        <v>16.14</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>40</v>
+      <c r="C8" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="16">
+      <c r="B9" s="12">
         <v>16.21</v>
       </c>
-      <c r="C9" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="D9" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="E9" s="19">
-        <v>16.239999999999998</v>
-      </c>
-      <c r="F9" s="17" t="s">
-        <v>38</v>
+      <c r="C9" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="16">
+      <c r="B10" s="12">
         <v>16.309999999999999</v>
       </c>
-      <c r="C10" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="D10" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="E10" s="19">
-        <v>16.34</v>
-      </c>
-      <c r="F10" s="23">
+      <c r="C10" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" s="17">
         <v>16.350000000000001</v>
       </c>
     </row>
@@ -830,19 +796,16 @@
       <c r="A11" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="11">
+      <c r="B11" s="12">
         <v>16.41</v>
       </c>
-      <c r="C11" s="19">
-        <v>16.420000000000002</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E11" s="19">
+      <c r="C11" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="15">
         <v>16.440000000000001</v>
       </c>
-      <c r="F11" s="23">
+      <c r="E11" s="17">
         <v>16.45</v>
       </c>
     </row>
@@ -850,19 +813,16 @@
       <c r="A12" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="16">
+      <c r="B12" s="12">
         <v>16.510000000000002</v>
       </c>
-      <c r="C12" s="19">
-        <v>16.52</v>
-      </c>
-      <c r="D12" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="E12" s="19">
+      <c r="C12" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="15">
         <v>16.54</v>
       </c>
-      <c r="F12" s="23">
+      <c r="E12" s="17">
         <v>16.55</v>
       </c>
     </row>
@@ -870,19 +830,16 @@
       <c r="A13" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="11">
+      <c r="B13" s="18">
         <v>16.61</v>
       </c>
-      <c r="C13" s="19">
-        <v>16.62</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E13" s="19">
+      <c r="C13" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="15">
         <v>16.64</v>
       </c>
-      <c r="F13" s="23">
+      <c r="E13" s="17">
         <v>16.649999999999999</v>
       </c>
     </row>
@@ -890,39 +847,33 @@
       <c r="A14" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="24">
+      <c r="B14" s="18">
         <v>16.71</v>
       </c>
-      <c r="C14" s="19">
-        <v>16.72</v>
-      </c>
-      <c r="D14" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="E14" s="19">
+      <c r="C14" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" s="15">
         <v>16.739999999999998</v>
       </c>
-      <c r="F14" s="23">
+      <c r="E14" s="17">
         <v>16.75</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="11">
+      <c r="B15" s="12">
         <v>16.809999999999999</v>
       </c>
-      <c r="C15" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="E15" s="19">
-        <v>16.84</v>
-      </c>
-      <c r="F15" s="23">
+      <c r="C15" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E15" s="17">
         <v>16.850000000000001</v>
       </c>
     </row>
@@ -930,64 +881,61 @@
       <c r="A16" t="s">
         <v>10</v>
       </c>
-      <c r="B16" s="12">
+      <c r="B16" s="21">
         <v>16.91</v>
       </c>
-      <c r="C16" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="D16" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="E16" s="25">
+      <c r="C16" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16" s="19">
         <v>16.940000000000001</v>
       </c>
-      <c r="F16" s="26">
+      <c r="E16" s="20">
         <v>16.95</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" s="5"/>
+      <c r="C20" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B20" s="6"/>
-      <c r="C20" s="5" t="s">
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21" s="6"/>
+      <c r="C21" s="4" t="s">
         <v>18</v>
-      </c>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B21" s="7"/>
-      <c r="C21" s="5" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22" s="2"/>
-      <c r="C22" s="5" t="s">
+      <c r="C22" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B23" s="10"/>
+      <c r="C23" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B23" s="14"/>
-      <c r="C23" s="5" t="s">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B24" s="7"/>
+      <c r="C24" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B24" s="8"/>
-      <c r="C24" s="5" t="s">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B25" s="8"/>
+      <c r="C25" s="4" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B25" s="9"/>
-      <c r="C25" s="5" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
WildCard matrix en EG regressie set bijgewerkt
</commit_message>
<xml_diff>
--- a/Testen/WildCard matrix.xlsx
+++ b/Testen/WildCard matrix.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="97">
   <si>
     <t>WildCard matrix</t>
   </si>
@@ -39,21 +39,12 @@
     <t>Clock</t>
   </si>
   <si>
-    <t>Timer</t>
-  </si>
-  <si>
-    <t>Variable</t>
-  </si>
-  <si>
     <t>EventList</t>
   </si>
   <si>
     <t>System</t>
   </si>
   <si>
-    <t>Event</t>
-  </si>
-  <si>
     <t>Unknown</t>
   </si>
   <si>
@@ -69,9 +60,6 @@
     <t>Legenda:</t>
   </si>
   <si>
-    <t>geldig, moet voorkomen bij alle geldige andere testcases in die rij/kolom.</t>
-  </si>
-  <si>
     <t>ongeldig, hoeft niet getest te worden</t>
   </si>
   <si>
@@ -87,74 +75,245 @@
     <t>onduidelijk, heeft uitleg nodig, of testcase onduidelijk</t>
   </si>
   <si>
-    <t xml:space="preserve">16,13
-inkomend signaal </t>
-  </si>
-  <si>
-    <t xml:space="preserve">16,23
-inkomend signaal </t>
-  </si>
-  <si>
-    <t xml:space="preserve">16,33
-inkomend signaal </t>
-  </si>
-  <si>
-    <t>16,43
-status wijziging</t>
-  </si>
-  <si>
-    <t>16,53
-zozo events</t>
-  </si>
-  <si>
-    <t>16,63
-timer loopt af</t>
-  </si>
-  <si>
-    <t>16,73
-variable wijzigt waarde</t>
-  </si>
-  <si>
-    <t>16,25
-inkomend signaal, maar bestemd voor andere unit</t>
-  </si>
-  <si>
     <t>De nummers in de cellen refereren aan de gegenereerde UserEvents in testcase 16</t>
   </si>
   <si>
-    <t>16,15
-inkomend signaal, maar bestemd voor andere unit</t>
-  </si>
-  <si>
-    <t>16,84
-hex value uit eventlist</t>
-  </si>
-  <si>
-    <t>16,83
-UserEvent</t>
-  </si>
-  <si>
-    <t>16,93
-boot</t>
-  </si>
-  <si>
-    <t>16,14
-inkomend signaal</t>
-  </si>
-  <si>
-    <t>16,24
-hex value uit RF</t>
-  </si>
-  <si>
-    <t>16,34
-hex value uit Serial</t>
+    <t>KAKU</t>
+  </si>
+  <si>
+    <t>NewKAKU</t>
+  </si>
+  <si>
+    <t>Error</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>UserEvent</t>
+  </si>
+  <si>
+    <t>16,01</t>
+  </si>
+  <si>
+    <t>16,02</t>
+  </si>
+  <si>
+    <t>16,03</t>
+  </si>
+  <si>
+    <t>16,04</t>
+  </si>
+  <si>
+    <t>16,05</t>
+  </si>
+  <si>
+    <t>16,06</t>
+  </si>
+  <si>
+    <t>16,07</t>
+  </si>
+  <si>
+    <t>16,08</t>
+  </si>
+  <si>
+    <t>16,12</t>
+  </si>
+  <si>
+    <t>16,13</t>
+  </si>
+  <si>
+    <t>16,14</t>
+  </si>
+  <si>
+    <t>16,15</t>
+  </si>
+  <si>
+    <t>16,16</t>
+  </si>
+  <si>
+    <t>16,17</t>
+  </si>
+  <si>
+    <t>16,18</t>
+  </si>
+  <si>
+    <t>16,23</t>
+  </si>
+  <si>
+    <t>16,24</t>
+  </si>
+  <si>
+    <t>16,25</t>
+  </si>
+  <si>
+    <t>16,27</t>
+  </si>
+  <si>
+    <t>16,28</t>
+  </si>
+  <si>
+    <t>16,22</t>
+  </si>
+  <si>
+    <t>16,32</t>
+  </si>
+  <si>
+    <t>16,33</t>
+  </si>
+  <si>
+    <t>16,34</t>
+  </si>
+  <si>
+    <t>16,35</t>
+  </si>
+  <si>
+    <t>16,36</t>
+  </si>
+  <si>
+    <t>16,37</t>
+  </si>
+  <si>
+    <t>16,38</t>
+  </si>
+  <si>
+    <t>16,42</t>
+  </si>
+  <si>
+    <t>16,43</t>
+  </si>
+  <si>
+    <t>16,44</t>
+  </si>
+  <si>
+    <t>16,45</t>
+  </si>
+  <si>
+    <t>16,46</t>
+  </si>
+  <si>
+    <t>16,47</t>
+  </si>
+  <si>
+    <t>16,48</t>
+  </si>
+  <si>
+    <t>16,52</t>
+  </si>
+  <si>
+    <t>16,53</t>
+  </si>
+  <si>
+    <t>16,54</t>
+  </si>
+  <si>
+    <t>16,55</t>
+  </si>
+  <si>
+    <t>16,56</t>
+  </si>
+  <si>
+    <t>16,57</t>
+  </si>
+  <si>
+    <t>16,58</t>
+  </si>
+  <si>
+    <t>16,62</t>
+  </si>
+  <si>
+    <t>16,63</t>
+  </si>
+  <si>
+    <t>16,64</t>
+  </si>
+  <si>
+    <t>16,65</t>
+  </si>
+  <si>
+    <t>16,66</t>
+  </si>
+  <si>
+    <t>16,67</t>
+  </si>
+  <si>
+    <t>16,68</t>
+  </si>
+  <si>
+    <t>16,72</t>
+  </si>
+  <si>
+    <t>16,73</t>
+  </si>
+  <si>
+    <t>16,74</t>
+  </si>
+  <si>
+    <t>16,75</t>
+  </si>
+  <si>
+    <t>16,76</t>
+  </si>
+  <si>
+    <t>16,77</t>
+  </si>
+  <si>
+    <t>16,78</t>
+  </si>
+  <si>
+    <t>16,82</t>
+  </si>
+  <si>
+    <t>16,83</t>
+  </si>
+  <si>
+    <t>16,84</t>
+  </si>
+  <si>
+    <t>16,85</t>
+  </si>
+  <si>
+    <t>16,86</t>
+  </si>
+  <si>
+    <t>16,87</t>
+  </si>
+  <si>
+    <t>16,88</t>
+  </si>
+  <si>
+    <t>16,92</t>
+  </si>
+  <si>
+    <t>16,93</t>
+  </si>
+  <si>
+    <t>16,94</t>
+  </si>
+  <si>
+    <t>16,95</t>
+  </si>
+  <si>
+    <t>16,96</t>
+  </si>
+  <si>
+    <t>16,97</t>
+  </si>
+  <si>
+    <t>16,98</t>
+  </si>
+  <si>
+    <t>Timers</t>
+  </si>
+  <si>
+    <t>Variables</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -177,26 +336,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -315,7 +461,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -327,58 +473,52 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -682,264 +822,394 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="6" width="30.7109375" style="1" customWidth="1"/>
+    <col min="2" max="9" width="19.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="9">
-        <v>16.100000000000001</v>
-      </c>
-      <c r="C7" s="11">
-        <v>16.3</v>
-      </c>
-      <c r="D7" s="11">
-        <v>16.399999999999999</v>
-      </c>
-      <c r="E7" s="16">
-        <v>16.5</v>
-      </c>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-    </row>
-    <row r="8" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="B7" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H7" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="I7" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="12">
+      <c r="B8" s="11">
         <v>16.11</v>
       </c>
-      <c r="C8" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" s="10" t="s">
+      <c r="C8" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E8" s="13" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="G8" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="I8" s="12" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="12">
+      <c r="B9" s="11">
         <v>16.21</v>
       </c>
-      <c r="C9" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="E9" s="13" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="C9" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G9" s="9">
+        <v>16.260000000000002</v>
+      </c>
+      <c r="H9" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="I9" s="12" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="12">
+      <c r="B10" s="11">
         <v>16.309999999999999</v>
       </c>
-      <c r="C10" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="E10" s="17">
-        <v>16.350000000000001</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="C10" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="I10" s="12" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="12">
+      <c r="B11" s="11">
         <v>16.41</v>
       </c>
-      <c r="C11" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="D11" s="15">
-        <v>16.440000000000001</v>
-      </c>
-      <c r="E11" s="17">
-        <v>16.45</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="C11" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="I11" s="17" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="12">
+      <c r="B12" s="16">
         <v>16.510000000000002</v>
       </c>
-      <c r="C12" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="D12" s="15">
-        <v>16.54</v>
-      </c>
-      <c r="E12" s="17">
-        <v>16.55</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="C12" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="I12" s="17" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>95</v>
+      </c>
+      <c r="B13" s="11">
+        <v>16.61</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="I13" s="17" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>96</v>
+      </c>
+      <c r="B14" s="11">
+        <v>16.71</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="I14" s="17" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="18">
-        <v>16.61</v>
-      </c>
-      <c r="C13" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="D13" s="15">
-        <v>16.64</v>
-      </c>
-      <c r="E13" s="17">
-        <v>16.649999999999999</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="B15" s="11">
+        <v>16.809999999999999</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="I15" s="12" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="18">
-        <v>16.71</v>
-      </c>
-      <c r="C14" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="D14" s="15">
-        <v>16.739999999999998</v>
-      </c>
-      <c r="E14" s="17">
-        <v>16.75</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>9</v>
-      </c>
-      <c r="B15" s="12">
-        <v>16.809999999999999</v>
-      </c>
-      <c r="C15" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="D15" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="E15" s="17">
-        <v>16.850000000000001</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>10</v>
-      </c>
-      <c r="B16" s="21">
+      <c r="B16" s="14">
         <v>16.91</v>
       </c>
-      <c r="C16" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="D16" s="19">
-        <v>16.940000000000001</v>
-      </c>
-      <c r="E16" s="20">
-        <v>16.95</v>
-      </c>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C16" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="D16" s="20" t="s">
+        <v>89</v>
+      </c>
+      <c r="E16" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="F16" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="G16" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="H16" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="I16" s="19" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20" s="5"/>
       <c r="C20" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B21" s="2"/>
+      <c r="C21" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B22" s="9"/>
+      <c r="C22" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B23" s="6"/>
+      <c r="C23" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B21" s="6"/>
-      <c r="C21" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B22" s="2"/>
-      <c r="C22" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B23" s="10"/>
-      <c r="C23" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B24" s="7"/>
       <c r="C24" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B25" s="8"/>
-      <c r="C25" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B26" s="2"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
regressieset en wildcard matrix aangepast
</commit_message>
<xml_diff>
--- a/Testen/WildCard matrix.xlsx
+++ b/Testen/WildCard matrix.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="95">
   <si>
     <t>WildCard matrix</t>
   </si>
@@ -72,9 +72,6 @@
     <t>geldig maar komt niet goed uit de test</t>
   </si>
   <si>
-    <t>onduidelijk, heeft uitleg nodig, of testcase onduidelijk</t>
-  </si>
-  <si>
     <t>De nummers in de cellen refereren aan de gegenereerde UserEvents in testcase 16</t>
   </si>
   <si>
@@ -177,9 +174,6 @@
     <t>16,38</t>
   </si>
   <si>
-    <t>16,42</t>
-  </si>
-  <si>
     <t>16,43</t>
   </si>
   <si>
@@ -304,6 +298,9 @@
   </si>
   <si>
     <t>Variables</t>
+  </si>
+  <si>
+    <t>Is altijd een "event", dus geen sub-classificatie nodig. Altijd afvangen met "All"</t>
   </si>
 </sst>
 </file>
@@ -366,7 +363,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -434,31 +431,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -501,21 +478,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -822,7 +784,7 @@
   <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -850,19 +812,19 @@
         <v>1</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>24</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>10</v>
@@ -876,28 +838,28 @@
         <v>1</v>
       </c>
       <c r="B7" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="D7" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="15" t="s">
+      <c r="E7" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="15" t="s">
+      <c r="F7" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="F7" s="15" t="s">
+      <c r="G7" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="G7" s="10" t="s">
+      <c r="H7" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="H7" s="10" t="s">
+      <c r="I7" s="13" t="s">
         <v>31</v>
-      </c>
-      <c r="I7" s="13" t="s">
-        <v>32</v>
       </c>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
@@ -910,25 +872,25 @@
         <v>16.11</v>
       </c>
       <c r="C8" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="E8" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="F8" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="G8" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="G8" s="9" t="s">
+      <c r="H8" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="I8" s="12" t="s">
         <v>38</v>
-      </c>
-      <c r="I8" s="12" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -939,25 +901,25 @@
         <v>16.21</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D9" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="F9" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>42</v>
       </c>
       <c r="G9" s="9">
         <v>16.260000000000002</v>
       </c>
       <c r="H9" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="I9" s="12" t="s">
         <v>43</v>
-      </c>
-      <c r="I9" s="17" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -968,25 +930,25 @@
         <v>16.309999999999999</v>
       </c>
       <c r="C10" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="E10" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="F10" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="G10" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="G10" s="9" t="s">
+      <c r="H10" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="H10" s="2" t="s">
+      <c r="I10" s="12" t="s">
         <v>51</v>
-      </c>
-      <c r="I10" s="12" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -996,113 +958,113 @@
       <c r="B11" s="11">
         <v>16.41</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="7">
+        <v>16.420000000000002</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="E11" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="F11" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="G11" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="H11" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="G11" s="5" t="s">
+      <c r="I11" s="7" t="s">
         <v>57</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="I11" s="17" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="16">
+      <c r="B12" s="11">
         <v>16.510000000000002</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="E12" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="F12" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="G12" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="H12" s="7">
+        <v>16.57</v>
+      </c>
+      <c r="I12" s="7" t="s">
         <v>63</v>
-      </c>
-      <c r="G12" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="H12" s="2">
-        <v>16.57</v>
-      </c>
-      <c r="I12" s="17" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B13" s="11">
         <v>16.61</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="E13" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="F13" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="G13" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="H13" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="G13" s="5" t="s">
+      <c r="I13" s="7" t="s">
         <v>70</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="I13" s="17" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B14" s="11">
         <v>16.71</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="E14" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="F14" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="G14" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="H14" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="G14" s="5" t="s">
+      <c r="I14" s="7" t="s">
         <v>77</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="I14" s="17" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -1113,25 +1075,25 @@
         <v>16.809999999999999</v>
       </c>
       <c r="C15" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E15" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="F15" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="G15" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="H15" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="G15" s="9" t="s">
+      <c r="I15" s="12" t="s">
         <v>84</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="I15" s="12" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1141,26 +1103,26 @@
       <c r="B16" s="14">
         <v>16.91</v>
       </c>
-      <c r="C16" s="20" t="s">
+      <c r="C16" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="E16" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="D16" s="20" t="s">
+      <c r="F16" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="E16" s="18" t="s">
+      <c r="G16" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="F16" s="18" t="s">
+      <c r="H16" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="G16" s="20" t="s">
+      <c r="I16" s="7" t="s">
         <v>91</v>
-      </c>
-      <c r="H16" s="18" t="s">
-        <v>92</v>
-      </c>
-      <c r="I16" s="19" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
@@ -1168,7 +1130,7 @@
         <v>13</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
@@ -1198,7 +1160,7 @@
     <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B24" s="7"/>
       <c r="C24" s="4" t="s">
-        <v>18</v>
+        <v>94</v>
       </c>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
regressieset aangepast. Tevens in documentatie WildCard mogelijkheden: de wildcard Eventlist, Unknown komt wel degelijk voor. Kleur aangepast.
</commit_message>
<xml_diff>
--- a/Testen/WildCard matrix.xlsx
+++ b/Testen/WildCard matrix.xlsx
@@ -117,16 +117,10 @@
     <t>16,17</t>
   </si>
   <si>
-    <t>16,23</t>
-  </si>
-  <si>
     <t>16,24</t>
   </si>
   <si>
     <t>16,25</t>
-  </si>
-  <si>
-    <t>16,28</t>
   </si>
   <si>
     <t>16,32</t>
@@ -322,6 +316,14 @@
   <si>
     <t>16,71
 change a variable</t>
+  </si>
+  <si>
+    <t>16,23
+Send NewKaku from remote Nodo</t>
+  </si>
+  <si>
+    <t>16,28
+unknown hex code (from temp sensor)</t>
   </si>
 </sst>
 </file>
@@ -817,7 +819,7 @@
   <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -876,7 +878,7 @@
       <c r="C7" s="8">
         <v>16.02</v>
       </c>
-      <c r="D7" s="15" t="s">
+      <c r="D7" s="9" t="s">
         <v>25</v>
       </c>
       <c r="E7" s="15" t="s">
@@ -905,7 +907,7 @@
         <v>16.11</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>29</v>
@@ -917,13 +919,13 @@
         <v>31</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>32</v>
       </c>
       <c r="I8" s="12" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -934,25 +936,25 @@
         <v>16.21</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="D9" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="F9" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="F9" s="2" t="s">
-        <v>35</v>
-      </c>
       <c r="G9" s="9" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="H9" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="I9" s="12" t="s">
-        <v>36</v>
+        <v>87</v>
+      </c>
+      <c r="I9" s="9" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -963,25 +965,25 @@
         <v>16.309999999999999</v>
       </c>
       <c r="C10" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="D10" s="16" t="s">
+      <c r="F10" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="E10" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="F10" s="16" t="s">
-        <v>40</v>
-      </c>
       <c r="G10" s="9" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H10" s="5">
         <v>16.37</v>
       </c>
-      <c r="I10" s="12" t="s">
-        <v>94</v>
+      <c r="I10" s="9" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -989,28 +991,28 @@
         <v>5</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C11" s="5">
         <v>16.420000000000002</v>
       </c>
       <c r="D11" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F11" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="G11" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="H11" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="G11" s="5" t="s">
+      <c r="I11" s="5" t="s">
         <v>44</v>
-      </c>
-      <c r="H11" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="I11" s="5" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -1018,86 +1020,86 @@
         <v>6</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C12" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E12" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="F12" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="G12" s="5" t="s">
         <v>49</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="G12" s="5" t="s">
-        <v>51</v>
       </c>
       <c r="H12" s="5">
         <v>16.57</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C13" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E13" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="F13" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="G13" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="H13" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="G13" s="5" t="s">
+      <c r="I13" s="5" t="s">
         <v>57</v>
-      </c>
-      <c r="H13" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="I13" s="5" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C14" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E14" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="F14" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="G14" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="F14" s="5" t="s">
+      <c r="H14" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="G14" s="5" t="s">
+      <c r="I14" s="5" t="s">
         <v>64</v>
-      </c>
-      <c r="H14" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="I14" s="5" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -1108,25 +1110,25 @@
         <v>16.809999999999999</v>
       </c>
       <c r="C15" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="D15" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="E15" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="D15" s="16" t="s">
+      <c r="F15" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="E15" s="16" t="s">
-        <v>69</v>
-      </c>
-      <c r="F15" s="16" t="s">
-        <v>70</v>
-      </c>
       <c r="G15" s="9" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="H15" s="5">
         <v>16.87</v>
       </c>
       <c r="I15" s="9" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1134,28 +1136,28 @@
         <v>8</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C16" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="E16" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="F16" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="E16" s="5" t="s">
+      <c r="G16" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="F16" s="5" t="s">
+      <c r="H16" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="G16" s="5" t="s">
+      <c r="I16" s="5" t="s">
         <v>75</v>
-      </c>
-      <c r="H16" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="I16" s="5" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
@@ -1193,13 +1195,13 @@
     <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B24" s="7"/>
       <c r="C24" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B25" s="16"/>
       <c r="C25" s="17" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>

</xml_diff>

<commit_message>
Wildcard matrix en regressieset aangepast. Nog 4 WildCard combinaties kunnen niet worden getest omdat geen testcase voorhanden is (Error en OK). Slechts 1 cel is rood, (zie issue)
</commit_message>
<xml_diff>
--- a/Testen/WildCard matrix.xlsx
+++ b/Testen/WildCard matrix.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="90">
   <si>
     <t>WildCard matrix</t>
   </si>
@@ -51,12 +51,6 @@
     <t>OtherUnit</t>
   </si>
   <si>
-    <t>Verticaal: par1, bron</t>
-  </si>
-  <si>
-    <t>Verticaal: par2, type</t>
-  </si>
-  <si>
     <t>Legenda:</t>
   </si>
   <si>
@@ -88,39 +82,6 @@
   </si>
   <si>
     <t>UserEvent</t>
-  </si>
-  <si>
-    <t>16,01</t>
-  </si>
-  <si>
-    <t>16,03</t>
-  </si>
-  <si>
-    <t>16,04</t>
-  </si>
-  <si>
-    <t>16,05</t>
-  </si>
-  <si>
-    <t>16,07</t>
-  </si>
-  <si>
-    <t>16,13</t>
-  </si>
-  <si>
-    <t>16,14</t>
-  </si>
-  <si>
-    <t>16,15</t>
-  </si>
-  <si>
-    <t>16,17</t>
-  </si>
-  <si>
-    <t>16,24</t>
-  </si>
-  <si>
-    <t>16,25</t>
   </si>
   <si>
     <t>16,32</t>
@@ -324,13 +285,38 @@
   <si>
     <t>16,28
 unknown hex code (from temp sensor)</t>
+  </si>
+  <si>
+    <t>16,17
+Send command for other unit from remote nodo via IR</t>
+  </si>
+  <si>
+    <t>16,13
+NewKAKU signal via IR from Harmony. 
+Problem: cannot learn NewKAKU into Harmony</t>
+  </si>
+  <si>
+    <t>16,14
+No testcase available</t>
+  </si>
+  <si>
+    <t>16,24
+No testcase available</t>
+  </si>
+  <si>
+    <t>16,15
+No testcase available</t>
+  </si>
+  <si>
+    <t>16,25
+No testcase available</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -349,6 +335,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -392,7 +384,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -401,60 +393,135 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top style="medium">
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top/>
-      <bottom/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -464,7 +531,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -485,28 +552,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -514,6 +560,48 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -816,10 +904,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K25"/>
+  <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -832,380 +920,376 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>11</v>
+    <row r="2" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="16">
+        <v>16.010000000000002</v>
+      </c>
+      <c r="C3" s="17">
+        <f>(B3+0.01)</f>
+        <v>16.020000000000003</v>
+      </c>
+      <c r="D3" s="17">
+        <f t="shared" ref="D3:H3" si="0">(C3+0.01)</f>
+        <v>16.030000000000005</v>
+      </c>
+      <c r="E3" s="17">
+        <f t="shared" si="0"/>
+        <v>16.040000000000006</v>
+      </c>
+      <c r="F3" s="17">
+        <f t="shared" si="0"/>
+        <v>16.050000000000008</v>
+      </c>
+      <c r="G3" s="17">
+        <f t="shared" si="0"/>
+        <v>16.060000000000009</v>
+      </c>
+      <c r="H3" s="17">
+        <f t="shared" si="0"/>
+        <v>16.070000000000011</v>
+      </c>
+      <c r="I3" s="18">
+        <v>16.079999999999998</v>
+      </c>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+    </row>
+    <row r="4" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="19">
+        <v>16.11</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="I4" s="20" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="19">
+        <v>16.21</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="I5" s="20" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="19">
+        <v>16.309999999999999</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="H6" s="15">
+        <v>16.37</v>
+      </c>
+      <c r="I6" s="20" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="C7" s="15">
+        <v>16.420000000000002</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="G7" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="H7" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="I7" s="21" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="G8" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="H8" s="15">
+        <v>16.57</v>
+      </c>
+      <c r="I8" s="21" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>63</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="F9" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="G9" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="H9" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="I9" s="21" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>64</v>
+      </c>
+      <c r="B10" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="F10" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="G10" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="H10" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="I10" s="21" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="19">
+        <v>16.809999999999999</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="F11" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="H11" s="15">
+        <v>16.87</v>
+      </c>
+      <c r="I11" s="20" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="C12" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="D12" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="E12" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="F12" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="G12" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="H12" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="I12" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B15" s="5"/>
+      <c r="C15" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" s="8">
-        <v>16.02</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="E7" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="F7" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="G7" s="10">
-        <v>16.059999999999999</v>
-      </c>
-      <c r="H7" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="I7" s="13">
-        <v>16.079999999999998</v>
-      </c>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-    </row>
-    <row r="8" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" s="11">
-        <v>16.11</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="G8" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="I8" s="12" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9" s="11">
-        <v>16.21</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="G9" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="H9" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="I9" s="9" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" s="11">
-        <v>16.309999999999999</v>
-      </c>
-      <c r="C10" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="D10" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="E10" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="F10" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="G10" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="H10" s="5">
-        <v>16.37</v>
-      </c>
-      <c r="I10" s="9" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="C11" s="5">
-        <v>16.420000000000002</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="H11" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="I11" s="5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="G12" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="H12" s="5">
-        <v>16.57</v>
-      </c>
-      <c r="I12" s="5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>76</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="H13" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="I13" s="5" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>77</v>
-      </c>
-      <c r="B14" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="G14" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="H14" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="I14" s="5" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>7</v>
-      </c>
-      <c r="B15" s="11">
-        <v>16.809999999999999</v>
-      </c>
-      <c r="C15" s="16" t="s">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B16" s="2"/>
+      <c r="C16" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B17" s="8"/>
+      <c r="C17" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B18" s="6"/>
+      <c r="C18" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B19" s="7"/>
+      <c r="C19" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="D15" s="16" t="s">
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B20" s="9"/>
+      <c r="C20" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="E15" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="F15" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="G15" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="H15" s="5">
-        <v>16.87</v>
-      </c>
-      <c r="I15" s="9" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>8</v>
-      </c>
-      <c r="B16" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="G16" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="H16" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="I16" s="5" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B19" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B20" s="5"/>
-      <c r="C20" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B21" s="2"/>
-      <c r="C21" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B22" s="9"/>
-      <c r="C22" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B23" s="6"/>
-      <c r="C23" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B24" s="7"/>
-      <c r="C24" s="4" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B25" s="16"/>
-      <c r="C25" s="17" t="s">
-        <v>79</v>
-      </c>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>